<commit_message>
new reports in excel sheet
</commit_message>
<xml_diff>
--- a/src/main/java/com/abhi/data/TcRAReportList.xlsx
+++ b/src/main/java/com/abhi/data/TcRAReportList.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>ReportName</t>
   </si>
@@ -39,18 +39,9 @@
     <t>ExpectedRows</t>
   </si>
   <si>
-    <t>Comment Status (Project)</t>
-  </si>
-  <si>
     <t>Document Status (Project)</t>
   </si>
   <si>
-    <t>Document Dashboard</t>
-  </si>
-  <si>
-    <t>PROJECT_13062018</t>
-  </si>
-  <si>
     <t>FilterKey</t>
   </si>
   <si>
@@ -63,25 +54,43 @@
     <t>[MYSELF]</t>
   </si>
   <si>
-    <t>Portfolio Status Tracker</t>
-  </si>
-  <si>
-    <t>Comment Status</t>
-  </si>
-  <si>
     <t>Document Status</t>
   </si>
   <si>
-    <t>Project Finance Structure Overview</t>
-  </si>
-  <si>
     <t>Project Teamcenter ID</t>
   </si>
   <si>
     <t>Project Tracker</t>
   </si>
   <si>
-    <t>316837*</t>
+    <t>Comment Status Internal (Project)</t>
+  </si>
+  <si>
+    <t>Project Invoice Overview (Project)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Document Dashboard (Project)</t>
+  </si>
+  <si>
+    <t>Comment Status Internal</t>
+  </si>
+  <si>
+    <t>Project Organization Overview</t>
+  </si>
+  <si>
+    <t>Project Portfolio Report</t>
+  </si>
+  <si>
+    <t>Comment Status External</t>
+  </si>
+  <si>
+    <t>Project Invoice Overview</t>
+  </si>
+  <si>
+    <t>312498*</t>
   </si>
 </sst>
 </file>
@@ -431,16 +440,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.25" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -457,10 +466,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -468,10 +477,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -479,13 +488,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -496,10 +516,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -515,10 +535,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -526,13 +546,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -540,27 +560,27 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -568,13 +588,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -582,15 +602,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>